<commit_message>
done with excel parse 0.1
</commit_message>
<xml_diff>
--- a/examples/dataset.xlsx
+++ b/examples/dataset.xlsx
@@ -15,32 +15,162 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>UniqueIdentifier,creator,date,title,description,coverage,subject,subject,publisher,identifier,format</t>
-  </si>
-  <si>
-    <t>WFG001000001_024,Jan Jansen,1732-01-15,Map of Amsterdam,"City and surrounding, including a nice illustration of the harbor",Amsterdam,city overview,harbor, blauw,WFG001000001_024.jpg,image/jpg</t>
-  </si>
-  <si>
-    <t>WFG001000001_025,Piet Hein,1768-06-27,Map of Gouda,Extensive map of Gouda with detailed legend,Gouda,city overview,, blauw,WFG001000001_025.jpg,image/jpg</t>
-  </si>
-  <si>
-    <t>WFG001000001_026,Jan Smit,1801-03-19,Map of Rotterdam,City overview with illustrated canals,Rotterdam,city overview,, blauw,WFG001000001_026.jpg,image/jpg</t>
-  </si>
-  <si>
-    <t>WFG001000001_027,Koning Keizer,1701-02-08,Map of Gorinchem,City surrounded with defensive star structure,Gorinchem,city overview,harbor, blauw,WFG001000001_027.jpg,image/jpg</t>
-  </si>
-  <si>
-    <t>WFG001000001_028,Willem de Vliet,1698-05-20,encyclopediapage of Schiedam,2 pages depicting Schiedam and its harbor area,Schiedam,city overview,, blauw,WFG001000001_028.jpg,image/jpg</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+  <si>
+    <t>UniqueIdentifier</t>
+  </si>
+  <si>
+    <t>creator</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>coverage</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>WFG001000001_024</t>
+  </si>
+  <si>
+    <t>Jan Jansen</t>
+  </si>
+  <si>
+    <t>1732-01-15</t>
+  </si>
+  <si>
+    <t>Map of Amsterdam</t>
+  </si>
+  <si>
+    <t>City and surrounding, including a nice illustration of the harbor</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>city overview</t>
+  </si>
+  <si>
+    <t>harbor</t>
+  </si>
+  <si>
+    <t> blauw</t>
+  </si>
+  <si>
+    <t>WFG001000001_024.jpg</t>
+  </si>
+  <si>
+    <t>image/jpg</t>
+  </si>
+  <si>
+    <t>WFG001000001_025</t>
+  </si>
+  <si>
+    <t>Piet Hein</t>
+  </si>
+  <si>
+    <t>1768-06-27</t>
+  </si>
+  <si>
+    <t>Map of Gouda</t>
+  </si>
+  <si>
+    <t>Extensive map of Gouda with detailed legend</t>
+  </si>
+  <si>
+    <t>Gouda</t>
+  </si>
+  <si>
+    <t>WFG001000001_025.jpg</t>
+  </si>
+  <si>
+    <t>WFG001000001_026</t>
+  </si>
+  <si>
+    <t>Jan Smit</t>
+  </si>
+  <si>
+    <t>1801-03-19</t>
+  </si>
+  <si>
+    <t>Map of Rotterdam</t>
+  </si>
+  <si>
+    <t>City overview with illustrated canals</t>
+  </si>
+  <si>
+    <t>Rotterdam</t>
+  </si>
+  <si>
+    <t>WFG001000001_026.jpg</t>
+  </si>
+  <si>
+    <t>WFG001000001_027</t>
+  </si>
+  <si>
+    <t>Koning Keizer</t>
+  </si>
+  <si>
+    <t>1701-02-08</t>
+  </si>
+  <si>
+    <t>Map of Gorinchem</t>
+  </si>
+  <si>
+    <t>City surrounded with defensive star structure</t>
+  </si>
+  <si>
+    <t>Gorinchem</t>
+  </si>
+  <si>
+    <t>WFG001000001_027.jpg</t>
+  </si>
+  <si>
+    <t>WFG001000001_028</t>
+  </si>
+  <si>
+    <t>Willem de Vliet</t>
+  </si>
+  <si>
+    <t>1698-05-20</t>
+  </si>
+  <si>
+    <t>encyclopediapage of Schiedam</t>
+  </si>
+  <si>
+    <t>2 pages depicting Schiedam and its harbor area</t>
+  </si>
+  <si>
+    <t>Schiedam</t>
+  </si>
+  <si>
+    <t>WFG001000001_028.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -106,8 +236,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -128,46 +262,227 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="165.591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.4489795918367"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="50.765306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.8163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="7.19897959183674"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="8.78571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.6173469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>35</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>42</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>